<commit_message>
incluido arquivos da pos ead de date warehouse e atualizado lista de cursos unibb
</commit_message>
<xml_diff>
--- a/CursosBB-2021.xlsx
+++ b/CursosBB-2021.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cezar\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projetos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>EDUCA</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>FEITO</t>
+  </si>
+  <si>
+    <t>V</t>
   </si>
 </sst>
 </file>
@@ -451,7 +454,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,6 +482,9 @@
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -487,6 +493,9 @@
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="C3" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -520,12 +529,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7781</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -542,6 +554,9 @@
       </c>
       <c r="B10" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualizado lista de gastos e planilha de cursos bb
</commit_message>
<xml_diff>
--- a/CursosBB-2021.xlsx
+++ b/CursosBB-2021.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>EDUCA</t>
   </si>
@@ -454,7 +454,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,6 +527,9 @@
       </c>
       <c r="B7" s="3" t="s">
         <v>7</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
atualizado planilha de gastos e lista de cursos unibb
</commit_message>
<xml_diff>
--- a/CursosBB-2021.xlsx
+++ b/CursosBB-2021.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>EDUCA</t>
   </si>
@@ -454,7 +454,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,6 +503,9 @@
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
atualizado lista de cursos unibb
</commit_message>
<xml_diff>
--- a/CursosBB-2021.xlsx
+++ b/CursosBB-2021.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>EDUCA</t>
   </si>
@@ -454,7 +454,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,6 +552,9 @@
       </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
atualizado planilha de cursos
</commit_message>
<xml_diff>
--- a/CursosBB-2021.xlsx
+++ b/CursosBB-2021.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projetos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cezar\projetos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>EDUCA</t>
   </si>
@@ -454,7 +454,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,6 +514,9 @@
       </c>
       <c r="B5" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>